<commit_message>
Added updating CB option
</commit_message>
<xml_diff>
--- a/main/new_companies.xlsx
+++ b/main/new_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG17"/>
+  <dimension ref="A1:BF17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,239 +506,234 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 14</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Full Description</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Full Description</t>
+          <t>CB (Crunchbase) Link</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>CB (Crunchbase) Link</t>
+          <t>Company CB Categories</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Company CB Categories</t>
+          <t>Company_Location</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Company_Location</t>
+          <t>Company_Founded_Year</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Company_Founded_Year</t>
+          <t>Company_Number_of_Employees</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Company_Number_of_Employees</t>
+          <t>Company_CB_Rank</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Company_CB_Rank</t>
+          <t>Funding_Status</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Funding_Status</t>
+          <t>Last_Funding_Type</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Last_Funding_Type</t>
+          <t>Last_Funding_Date</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Last_Funding_Date</t>
+          <t>Last_Funding_Amount</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Last_Funding_Amount</t>
+          <t>Total_Funding_Amount</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Total_Funding_Amount</t>
+          <t>Total_Funding_Amount_M_dollars</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>Total_Funding_Amount_M_dollars</t>
+          <t>Number_of_Funding_Rounds</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>Number_of_Funding_Rounds</t>
+          <t>Estimated_Revenue_Range</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>Estimated_Revenue_Range</t>
+          <t>Company_Number_of_Investors</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>Company_Number_of_Investors</t>
+          <t>Company_Number_of_Investments</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>Company_Number_of_Investments</t>
+          <t>Company LinkedIn Link</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>Company LinkedIn Link</t>
+          <t>Company_LinkedIn_Followers_Number</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>Company_LinkedIn_Followers_Number</t>
+          <t>Company Contact Email</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>Company Contact Email</t>
+          <t>Company phone number</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>Company phone number</t>
+          <t>Founders</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>Founders</t>
+          <t xml:space="preserve">CSO </t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">CSO </t>
+          <t>CTO</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>CTO</t>
+          <t>CEO</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>CEO</t>
+          <t>COO</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>COO</t>
+          <t>CFO</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>CFO</t>
+          <t>Co-Founder</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>Co-Founder</t>
+          <t>President</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>President</t>
+          <t>Team Members</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>Team Members</t>
+          <t>Address</t>
         </is>
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>Address</t>
+          <t>former company names</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>former company names</t>
+          <t>acquired</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>acquired</t>
+          <t>product_stage</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
         <is>
-          <t>product_stage</t>
+          <t xml:space="preserve">Number of Patents </t>
         </is>
       </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Number of Patents </t>
+          <t>Comments</t>
         </is>
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>Comments</t>
+          <t>Unnamed: 51</t>
         </is>
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 52</t>
+          <t>Contact Name</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
         <is>
-          <t>Contact Name</t>
+          <t>Contact Phone Number / Email</t>
         </is>
       </c>
       <c r="BC1" s="1" t="inlineStr">
         <is>
-          <t>Contact Phone Number / Email</t>
+          <t>האם יצרנו איתם כבר קשר? (כדי לא להתיש)</t>
         </is>
       </c>
       <c r="BD1" s="1" t="inlineStr">
         <is>
-          <t>האם יצרנו איתם כבר קשר? (כדי לא להתיש)</t>
+          <t>BrainstormIL contact</t>
         </is>
       </c>
       <c r="BE1" s="1" t="inlineStr">
         <is>
-          <t>BrainstormIL contact</t>
+          <t>Unnamed: 56</t>
         </is>
       </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 57</t>
-        </is>
-      </c>
-      <c r="BG1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 58</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dive</t>
+          <t>CardiaCare</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -746,41 +741,47 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>https://finder.startupnationcentral.org/company_page/dive-1</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>CardiaCare is a medical device for with neuromodulation therapy in AFib patients.</t>
+        </is>
+      </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Innovation for Psychology</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr"/>
+          <t>CardiaCare is a medical device for neuromodulation therapy in AFib patients.</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>https://www.crunchbase.com/organization/cardiacare</t>
+        </is>
+      </c>
       <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="n">
-        <v>2022</v>
-      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Ness Ziona, HaMerkaz, Israel</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>2018-01-01</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr">
         <is>
-          <t>1-10</t>
+          <t>101,741</t>
         </is>
       </c>
       <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>Pre-Funding</t>
-        </is>
-      </c>
+      <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
@@ -815,17 +816,16 @@
       <c r="BD2" t="inlineStr"/>
       <c r="BE2" t="inlineStr"/>
       <c r="BF2" t="inlineStr"/>
-      <c r="BG2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Enlight Exchange</t>
+          <t>Epitech</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -833,41 +833,47 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>https://finder.startupnationcentral.org/company_page/enlight-exchange</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Epitech is developing a Breakthrough Treatment For Dry Eye Syndrome.</t>
+        </is>
+      </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Global Mental Health Data Exchange</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr"/>
+          <t>Epitech is a developer of non-invasive ocular neurostimulation therapy, designed to treat the entire ocular surface and tear film, for long-lasting relief of dry eye symptoms. Its proprietary technology is based on neurostimulation by targeted magnetic fields, resulting in the reinforcement of the structural integrity of the ocular surface. Epitech the company was founded in 2015 and is based in Yokneam Illit, Israel.</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>https://www.crunchbase.com/organization/epitech-3</t>
+        </is>
+      </c>
       <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="n">
-        <v>2022</v>
-      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Yoqne`am `illit, HaZafon, Israel</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>2015-01-01</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr">
         <is>
-          <t>1-10</t>
+          <t>139,249</t>
         </is>
       </c>
       <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>Pre-Funding</t>
-        </is>
-      </c>
+      <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
@@ -902,17 +908,16 @@
       <c r="BD3" t="inlineStr"/>
       <c r="BE3" t="inlineStr"/>
       <c r="BF3" t="inlineStr"/>
-      <c r="BG3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MSICS Pharma</t>
+          <t>Aposense</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -920,41 +925,47 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>https://finder.startupnationcentral.org/company_page/msics-pharma</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Aposense is a molecular imaging and drug development company, with a pipeline of products, based on its apoptosis-based technology.</t>
+        </is>
+      </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Naturally sourced Psilocybin for Mental Healthcare</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr"/>
+          <t>Aposense (formerly NST) is a clinical-stage molecular imaging and drug development company, with a pipeline of products based on its patented platform technology for targeting apoptosis (programmed cell death) in vivo. The company translating the science of Apoptosis (programmed cell death) into personalized patient care in multiple disease categories, including oncology, cardiology, and neurology. Targeting of this important biological process in-vivo opens opportunities for real-time clinical imaging of disease activity and targeted therapy. Aposense specializing in the development of novel drugs and utilizing membrane electrical forces for trans-membrane of macromolecule drugs, mainly siRNA. It also developed rationally-designed molecular nano-motors (MNMs), being novel small-molecule chemical entities and its translation into kinetic energy for movement within the hydrophobic membrane core. Aposense was founded in 1996 and is headquartered in Petah Tiqva, HaMerkaz, Israel.</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>https://www.crunchbase.com/organization/aposense</t>
+        </is>
+      </c>
       <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="n">
-        <v>2022</v>
-      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Petah Tiqva, HaMerkaz, Israel</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>1996-01-01</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr">
         <is>
-          <t>1-10</t>
+          <t>250,425</t>
         </is>
       </c>
       <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>Pre-Funding</t>
-        </is>
-      </c>
+      <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr"/>
@@ -989,17 +1000,16 @@
       <c r="BD4" t="inlineStr"/>
       <c r="BE4" t="inlineStr"/>
       <c r="BF4" t="inlineStr"/>
-      <c r="BG4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Beffi</t>
+          <t>GG Apps</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -1007,41 +1017,47 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>https://finder.startupnationcentral.org/company_page/beffi</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>GG Apps specializes in providing cognitive behavioral therapy application.</t>
+        </is>
+      </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>AI-Based Companion for Elderly Brain Mental Health Support</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr"/>
+          <t>GG Apps specializes in providing cognitive behavioral therapy applications. The platform was created for the sole purpose of utilizing the latest mobile technologies for effective psychological training. The company was founded in 2016 and is headquartered in Tel Aviv, Israel.</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>https://www.crunchbase.com/organization/gg-apps</t>
+        </is>
+      </c>
       <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="n">
-        <v>2021</v>
-      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Tel Aviv, Tel Aviv, Israel</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>2016-01-01</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr">
         <is>
-          <t>1-10</t>
+          <t>574,625</t>
         </is>
       </c>
       <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>Pre-Funding</t>
-        </is>
-      </c>
+      <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="inlineStr"/>
@@ -1076,17 +1092,16 @@
       <c r="BD5" t="inlineStr"/>
       <c r="BE5" t="inlineStr"/>
       <c r="BF5" t="inlineStr"/>
-      <c r="BG5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CardiaCare</t>
+          <t>New Bio Technology</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -1101,39 +1116,35 @@
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>CardiaCare is a medical device for with neuromodulation therapy in AFib patients.</t>
-        </is>
-      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>New Bio Technology provides lab instrumentation for neuroscience research and tailors solutions for various research entities.</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>CardiaCare is a medical device for neuromodulation therapy in AFib patients.</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>https://www.crunchbase.com/organization/cardiacare</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr"/>
+          <t>https://www.crunchbase.com/organization/nbt-new-bio-technology</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Or Akiva, Hefa, Israel</t>
+        </is>
+      </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>Ness Ziona, HaMerkaz, Israel</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>2018-01-01</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>101,741</t>
-        </is>
-      </c>
+          <t>1992-01-01</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>653,014</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr"/>
@@ -1169,17 +1180,16 @@
       <c r="BD6" t="inlineStr"/>
       <c r="BE6" t="inlineStr"/>
       <c r="BF6" t="inlineStr"/>
-      <c r="BG6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Epitech</t>
+          <t>Corundum Neuroscience</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -1194,39 +1204,31 @@
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>Epitech is developing a Breakthrough Treatment For Dry Eye Syndrome.</t>
-        </is>
-      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Corundum Neuroscience is a research, venture building, and investment firm for neuroscience related projects.</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Epitech is a developer of non-invasive ocular neurostimulation therapy, designed to treat the entire ocular surface and tear film, for long-lasting relief of dry eye symptoms. Its proprietary technology is based on neurostimulation by targeted magnetic fields, resulting in the reinforcement of the structural integrity of the ocular surface. Epitech the company was founded in 2015 and is based in Yokneam Illit, Israel.</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>https://www.crunchbase.com/organization/epitech-3</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>Yoqne`am `illit, HaZafon, Israel</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>2015-01-01</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>139,249</t>
-        </is>
-      </c>
+          <t>https://www.crunchbase.com/organization/corundum-neuroscience</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Herzliya, Tel Aviv, Israel</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>991,149</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr"/>
@@ -1262,17 +1264,16 @@
       <c r="BD7" t="inlineStr"/>
       <c r="BE7" t="inlineStr"/>
       <c r="BF7" t="inlineStr"/>
-      <c r="BG7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Aposense</t>
+          <t>Synapse Research</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -1287,39 +1288,31 @@
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>Aposense is a molecular imaging and drug development company, with a pipeline of products, based on its apoptosis-based technology.</t>
-        </is>
-      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Synapse Research is a digital marketing agency that provides community management, web development, social media, and metaverse services.</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Aposense (formerly NST) is a clinical-stage molecular imaging and drug development company, with a pipeline of products based on its patented platform technology for targeting apoptosis (programmed cell death) in vivo. The company translating the science of Apoptosis (programmed cell death) into personalized patient care in multiple disease categories, including oncology, cardiology, and neurology. Targeting of this important biological process in-vivo opens opportunities for real-time clinical imaging of disease activity and targeted therapy. Aposense specializing in the development of novel drugs and utilizing membrane electrical forces for trans-membrane of macromolecule drugs, mainly siRNA. It also developed rationally-designed molecular nano-motors (MNMs), being novel small-molecule chemical entities and its translation into kinetic energy for movement within the hydrophobic membrane core. Aposense was founded in 1996 and is headquartered in Petah Tiqva, HaMerkaz, Israel.</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>https://www.crunchbase.com/organization/aposense</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>Petah Tiqva, HaMerkaz, Israel</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>1996-01-01</t>
-        </is>
-      </c>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>250,425</t>
-        </is>
-      </c>
+          <t>https://www.crunchbase.com/organization/synapse-research</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Tel Aviv, Tel Aviv, Israel</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>1,210,988</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr"/>
@@ -1355,17 +1348,16 @@
       <c r="BD8" t="inlineStr"/>
       <c r="BE8" t="inlineStr"/>
       <c r="BF8" t="inlineStr"/>
-      <c r="BG8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GG Apps</t>
+          <t>Clara Mind</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -1380,39 +1372,39 @@
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Clara Mind is a personalized tool for early identification of cognitive decline enabling remote monitoring of patients cognitive status.</t>
+        </is>
+      </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>GG Apps specializes in providing cognitive behavioral therapy application.</t>
+          <t>Clara Mind is a personalized tool for early identification of cognitive decline enabling remote monitoring of patient's cognitive status. This easy-to-use app enables remote monitoring of patients' cognitive status, thus bringing earlier care to care to patients and impacting the course of treatment. The tool brings care to patients before it is too late, impacting their treatment, healthcare systems, and drug development. Clara Mind saves valuable time for the doctor, as the patient can perform the test in the clinic waiting room, or even at home. The company compares your orientation performance to a large database of patients to provide your healthcare provider with critical information to help with your diagnosis and treatment.</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>GG Apps specializes in providing cognitive behavioral therapy applications. The platform was created for the sole purpose of utilizing the latest mobile technologies for effective psychological training. The company was founded in 2016 and is headquartered in Tel Aviv, Israel.</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>https://www.crunchbase.com/organization/gg-apps</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr"/>
+          <t>https://www.crunchbase.com/organization/clara-mind</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Tel Aviv, Tel Aviv, Israel</t>
+        </is>
+      </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>Tel Aviv, Tel Aviv, Israel</t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>2016-01-01</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>574,625</t>
-        </is>
-      </c>
+          <t>2016-09-01</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>1,274,195</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr"/>
@@ -1448,17 +1440,16 @@
       <c r="BD9" t="inlineStr"/>
       <c r="BE9" t="inlineStr"/>
       <c r="BF9" t="inlineStr"/>
-      <c r="BG9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>New Bio Technology</t>
+          <t>Lev Hasharon Mental Health Center</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -1473,35 +1464,31 @@
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>New Bio Technology provides lab instrumentation for neuroscience research and tailors solutions for various research entities.</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>https://www.crunchbase.com/organization/nbt-new-bio-technology</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>Or Akiva, Hefa, Israel</t>
-        </is>
-      </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>1992-01-01</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>653,014</t>
-        </is>
-      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Lev Hasharon Mental Health Center is a mental health center that offers psychiatry, psychology, and depression treatments.</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>https://www.crunchbase.com/organization/lev-hasharon-mental-health-center</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Tsur Moshe, HaMerkaz, Israel</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>1,521,471</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr"/>
@@ -1537,17 +1524,16 @@
       <c r="BD10" t="inlineStr"/>
       <c r="BE10" t="inlineStr"/>
       <c r="BF10" t="inlineStr"/>
-      <c r="BG10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Corundum Neuroscience</t>
+          <t>AvoMed</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -1562,31 +1548,35 @@
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>AvoMed specializes in focusing on Hematology, Neurology, Oncology, Rheumatology, and Dermatology with specific game-changing key products.</t>
+        </is>
+      </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Corundum Neuroscience is a research, venture building, and investment firm for neuroscience related projects.</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>https://www.crunchbase.com/organization/corundum-neuroscience</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>Herzliya, Tel Aviv, Israel</t>
-        </is>
-      </c>
+          <t>AvoMed specializes in focusing on Hematology, Neurology, Oncology, Rheumatology, and Dermatology with specific game-changing key products.</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>https://www.crunchbase.com/organization/avomed</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Tel Aviv, Tel Aviv, Israel</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>991,149</t>
-        </is>
-      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>1,653,087</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr"/>
@@ -1622,17 +1612,16 @@
       <c r="BD11" t="inlineStr"/>
       <c r="BE11" t="inlineStr"/>
       <c r="BF11" t="inlineStr"/>
-      <c r="BG11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Synapse Research</t>
+          <t>RGL Research</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -1647,31 +1636,39 @@
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Contract Research Organization</t>
+        </is>
+      </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Synapse Research is a digital marketing agency that provides community management, web development, social media, and metaverse services.</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>https://www.crunchbase.com/organization/synapse-research</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr"/>
+          <t>R.G.L Research is a contract research organization (CRO) providing expertise and reliable support to the pharmaceutical industries for conducting Clinical Trials. Our clients and partners include pharmaceuticals, biotechnologies, startups, academic and government organization. R.G.L Research is providing tailored and quality services to help clients and partners bend the cost and time curve of drug development to deliver new alternative product and innovative treatment to improve patients quality of life. R.G.L Research has vast professional experience and academic knowledge in performing clinical trials in Israel as well as developing health product in diverse therapeutic areas of medicine, in particular, neurology (Alzheimer, ALS, Multiple Sclerosis, Parkinson) and oncology (ovarian, colorectal cancer, T-Cell Lymphoma). Through its strong links and partnerships, R.G.L Research has become an international platform for clinical trials allowing its clients to reach patients from Israel, the United-States, France, Eastern Europe, NorthAfrica, ad India.</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>https://www.crunchbase.com/organization/rgl-research</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Tel Aviv, Tel Aviv, Israel</t>
+        </is>
+      </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>Tel Aviv, Tel Aviv, Israel</t>
+          <t>2015-01-01</t>
         </is>
       </c>
       <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>1,210,988</t>
-        </is>
-      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>2,692,900</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="inlineStr"/>
@@ -1707,17 +1704,16 @@
       <c r="BD12" t="inlineStr"/>
       <c r="BE12" t="inlineStr"/>
       <c r="BF12" t="inlineStr"/>
-      <c r="BG12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Clara Mind</t>
+          <t>PSYK-ed</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -1732,39 +1728,31 @@
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>Clara Mind is a personalized tool for early identification of cognitive decline enabling remote monitoring of patients cognitive status.</t>
-        </is>
-      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>PSYK-ed is a mental health company.</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Clara Mind is a personalized tool for early identification of cognitive decline enabling remote monitoring of patient's cognitive status. This easy-to-use app enables remote monitoring of patients' cognitive status, thus bringing earlier care to care to patients and impacting the course of treatment. The tool brings care to patients before it is too late, impacting their treatment, healthcare systems, and drug development. Clara Mind saves valuable time for the doctor, as the patient can perform the test in the clinic waiting room, or even at home. The company compares your orientation performance to a large database of patients to provide your healthcare provider with critical information to help with your diagnosis and treatment.</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>https://www.crunchbase.com/organization/clara-mind</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>Tel Aviv, Tel Aviv, Israel</t>
-        </is>
-      </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>2016-09-01</t>
-        </is>
-      </c>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>1,274,195</t>
-        </is>
-      </c>
+          <t>https://www.crunchbase.com/organization/psyk-ed</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Bet Shemesh, Yerushalayim, Israel</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>2,742,827</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="inlineStr"/>
@@ -1800,17 +1788,16 @@
       <c r="BD13" t="inlineStr"/>
       <c r="BE13" t="inlineStr"/>
       <c r="BF13" t="inlineStr"/>
-      <c r="BG13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Lev Hasharon Mental Health Center</t>
+          <t>Dive</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -1818,36 +1805,38 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>https://finder.startupnationcentral.org/company_page/dive-1</t>
+        </is>
+      </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>Lev Hasharon Mental Health Center is a mental health center that offers psychiatry, psychology, and depression treatments.</t>
-        </is>
-      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Innovation for Psychology</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>https://www.crunchbase.com/organization/lev-hasharon-mental-health-center</t>
-        </is>
-      </c>
+      <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>Tsur Moshe, HaMerkaz, Israel</t>
-        </is>
-      </c>
-      <c r="U14" t="inlineStr"/>
+      <c r="T14" t="n">
+        <v>2022</v>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>1-10</t>
+        </is>
+      </c>
       <c r="V14" t="inlineStr"/>
       <c r="W14" t="inlineStr">
         <is>
-          <t>1,521,471</t>
+          <t>Pre-Funding</t>
         </is>
       </c>
       <c r="X14" t="inlineStr"/>
@@ -1885,17 +1874,16 @@
       <c r="BD14" t="inlineStr"/>
       <c r="BE14" t="inlineStr"/>
       <c r="BF14" t="inlineStr"/>
-      <c r="BG14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>AvoMed</t>
+          <t>Enlight Exchange</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -1903,40 +1891,38 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>https://finder.startupnationcentral.org/company_page/enlight-exchange</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>AvoMed specializes in focusing on Hematology, Neurology, Oncology, Rheumatology, and Dermatology with specific game-changing key products.</t>
-        </is>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>AvoMed specializes in focusing on Hematology, Neurology, Oncology, Rheumatology, and Dermatology with specific game-changing key products.</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>https://www.crunchbase.com/organization/avomed</t>
-        </is>
-      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Global Mental Health Data Exchange</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>Tel Aviv, Tel Aviv, Israel</t>
-        </is>
-      </c>
-      <c r="U15" t="inlineStr"/>
+      <c r="T15" t="n">
+        <v>2022</v>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>1-10</t>
+        </is>
+      </c>
       <c r="V15" t="inlineStr"/>
       <c r="W15" t="inlineStr">
         <is>
-          <t>1,653,087</t>
+          <t>Pre-Funding</t>
         </is>
       </c>
       <c r="X15" t="inlineStr"/>
@@ -1974,17 +1960,16 @@
       <c r="BD15" t="inlineStr"/>
       <c r="BE15" t="inlineStr"/>
       <c r="BF15" t="inlineStr"/>
-      <c r="BG15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>RGL Research</t>
+          <t>MSICS Pharma</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -1992,44 +1977,38 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://finder.startupnationcentral.org/company_page/msics-pharma</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>Contract Research Organization</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>R.G.L Research is a contract research organization (CRO) providing expertise and reliable support to the pharmaceutical industries for conducting Clinical Trials. Our clients and partners include pharmaceuticals, biotechnologies, startups, academic and government organization. R.G.L Research is providing tailored and quality services to help clients and partners bend the cost and time curve of drug development to deliver new alternative product and innovative treatment to improve patients quality of life. R.G.L Research has vast professional experience and academic knowledge in performing clinical trials in Israel as well as developing health product in diverse therapeutic areas of medicine, in particular, neurology (Alzheimer, ALS, Multiple Sclerosis, Parkinson) and oncology (ovarian, colorectal cancer, T-Cell Lymphoma). Through its strong links and partnerships, R.G.L Research has become an international platform for clinical trials allowing its clients to reach patients from Israel, the United-States, France, Eastern Europe, NorthAfrica, ad India.</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>https://www.crunchbase.com/organization/rgl-research</t>
-        </is>
-      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Naturally sourced Psilocybin for Mental Healthcare</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>Tel Aviv, Tel Aviv, Israel</t>
-        </is>
+      <c r="T16" t="n">
+        <v>2022</v>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>2015-01-01</t>
+          <t>1-10</t>
         </is>
       </c>
       <c r="V16" t="inlineStr"/>
       <c r="W16" t="inlineStr">
         <is>
-          <t>2,692,900</t>
+          <t>Pre-Funding</t>
         </is>
       </c>
       <c r="X16" t="inlineStr"/>
@@ -2067,17 +2046,16 @@
       <c r="BD16" t="inlineStr"/>
       <c r="BE16" t="inlineStr"/>
       <c r="BF16" t="inlineStr"/>
-      <c r="BG16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PSYK-ed</t>
+          <t>Beffi</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>21-08-2024</t>
+          <t>23-08-2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -2085,36 +2063,38 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>https://finder.startupnationcentral.org/company_page/beffi</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>PSYK-ed is a mental health company.</t>
-        </is>
-      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>AI-Based Companion for Elderly Brain Mental Health Support</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>https://www.crunchbase.com/organization/psyk-ed</t>
-        </is>
-      </c>
+      <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t>Bet Shemesh, Yerushalayim, Israel</t>
-        </is>
-      </c>
-      <c r="U17" t="inlineStr"/>
+      <c r="T17" t="n">
+        <v>2021</v>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>1-10</t>
+        </is>
+      </c>
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr">
         <is>
-          <t>2,742,827</t>
+          <t>Pre-Funding</t>
         </is>
       </c>
       <c r="X17" t="inlineStr"/>
@@ -2152,7 +2132,6 @@
       <c r="BD17" t="inlineStr"/>
       <c r="BE17" t="inlineStr"/>
       <c r="BF17" t="inlineStr"/>
-      <c r="BG17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>